<commit_message>
updated Sprint & Journal for 2nd week
</commit_message>
<xml_diff>
--- a/HotelBookingApplication/files/Sprint/Sprint.xlsx
+++ b/HotelBookingApplication/files/Sprint/Sprint.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajup\Desktop\Sprint Sheets\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC55755-C718-44C9-91D8-A1E48B40EF70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33004647-9FC1-4609-BA52-82895F18126C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprint1" sheetId="1" r:id="rId1"/>
-    <sheet name="Burndown1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint1" sheetId="3" r:id="rId1"/>
+    <sheet name="Burndown1" sheetId="4" r:id="rId2"/>
+    <sheet name="Sprint2" sheetId="1" r:id="rId3"/>
+    <sheet name="Burndown2" sheetId="2" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +42,64 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+  <si>
+    <t>Week #2  (4 days / week)</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Task Owner</t>
+  </si>
+  <si>
+    <t>Initial Estimate (Total Sprint Hours = 24*1)</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>Environment Setup</t>
+  </si>
+  <si>
+    <t>Configure the project tech stack i.e ReactJS &amp; Node</t>
+  </si>
+  <si>
+    <t>Akhil</t>
+  </si>
+  <si>
+    <t>Sharan</t>
+  </si>
+  <si>
+    <t>Configure the project tech stack i.e ReactJS</t>
+  </si>
+  <si>
+    <t>Raju</t>
+  </si>
+  <si>
+    <t>Configure the project tech stack i.e MongoDB</t>
+  </si>
+  <si>
+    <t>Prerna</t>
+  </si>
+  <si>
+    <t>Team:</t>
+  </si>
+  <si>
+    <t>6 hours / Week</t>
+  </si>
+  <si>
+    <t>Total Available Hours During Sprint 2:</t>
+  </si>
   <si>
     <t>Week #1 (4 days / week)</t>
   </si>
@@ -47,27 +107,9 @@
     <t>Backlog Item</t>
   </si>
   <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>Task Owner</t>
-  </si>
-  <si>
     <t>Initial Estimate (Total Sprint Hours = 16*1)</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
     <t>28/2/2022</t>
   </si>
   <si>
@@ -83,28 +125,13 @@
     <t xml:space="preserve">Understand the requirements &amp; explore other hotel sites </t>
   </si>
   <si>
-    <t>Akhil</t>
-  </si>
-  <si>
     <t>Figure out the components</t>
   </si>
   <si>
-    <t>Sharan</t>
-  </si>
-  <si>
     <t>Figure out the technologies</t>
   </si>
   <si>
-    <t>Raju</t>
-  </si>
-  <si>
     <t>Figure out the pages design to be included</t>
-  </si>
-  <si>
-    <t>Prerna</t>
-  </si>
-  <si>
-    <t>Team:</t>
   </si>
   <si>
     <t>4 hours / Week</t>
@@ -120,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m&quot;/&quot;d"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,13 +174,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
@@ -165,6 +185,12 @@
       <i/>
       <sz val="9"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -189,6 +215,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -210,22 +243,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -259,6 +281,32 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -284,21 +332,6 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -337,6 +370,21 @@
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -394,91 +442,110 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -566,7 +633,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sprint1!$E$3:$H$3</c:f>
+              <c:f>[2]Sprint1!$E$3:$H$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -607,7 +674,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4792-43D5-8C80-2B415527D209}"/>
+              <c16:uniqueId val="{00000000-5195-4790-91E3-C8D57E4938BB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -631,7 +698,7 @@
           </c:spPr>
           <c:cat>
             <c:strRef>
-              <c:f>Sprint1!$E$3:$H$3</c:f>
+              <c:f>[2]Sprint1!$E$3:$H$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -651,7 +718,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sprint1!$E$5:$H$5</c:f>
+              <c:f>[2]Sprint1!$E$5:$H$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -672,7 +739,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4792-43D5-8C80-2B415527D209}"/>
+              <c16:uniqueId val="{00000001-5195-4790-91E3-C8D57E4938BB}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -861,11 +928,375 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1600" b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:rPr>
+              <a:t>Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal Burn Down </c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="3366CC">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sprint2!$E$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>m"/"d</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>44745</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44776</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44807</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44837</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]Sprint2!$E$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7945-45CB-97EB-BCCBC5526564}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual Burn Down</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="DC3912">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="DC3912"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sprint2!$E$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>m"/"d</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>44745</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44776</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44807</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44837</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint2!$E$5:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7945-45CB-97EB-BCCBC5526564}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="759426033"/>
+        <c:axId val="1662617950"/>
+      </c:areaChart>
+      <c:dateAx>
+        <c:axId val="759426033"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="m&quot;/&quot;d" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1662617950"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1662617950"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t>Remaining  Hours</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="759426033"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Roboto"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -876,7 +1307,45 @@
         <xdr:cNvPr id="2" name="Chart 1" title="Chart">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB4D20F2-198C-4D55-A99E-01876F73AF03}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BFEE298-686C-432C-851C-FA488AB96B2E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="9763125" cy="4914900"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 2" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C72E5036-31C6-40F2-BB42-D34BA0D2F7BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -926,20 +1395,6 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
-        <row r="3">
-          <cell r="E3" t="str">
-            <v>28/2/2022</v>
-          </cell>
-          <cell r="F3">
-            <v>44621</v>
-          </cell>
-          <cell r="G3">
-            <v>44622</v>
-          </cell>
-          <cell r="H3">
-            <v>44623</v>
-          </cell>
-        </row>
         <row r="4">
           <cell r="E4">
             <v>16</v>
@@ -954,23 +1409,52 @@
             <v>0</v>
           </cell>
         </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="3">
+          <cell r="E3">
+            <v>44745</v>
+          </cell>
+          <cell r="F3">
+            <v>44776</v>
+          </cell>
+          <cell r="G3">
+            <v>44807</v>
+          </cell>
+          <cell r="H3">
+            <v>44837</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="E4">
+            <v>24</v>
+          </cell>
+          <cell r="F4">
+            <v>15</v>
+          </cell>
+          <cell r="G4">
+            <v>7</v>
+          </cell>
+          <cell r="H4">
+            <v>0</v>
+          </cell>
+        </row>
         <row r="5">
           <cell r="E5">
-            <v>16</v>
+            <v>24</v>
           </cell>
           <cell r="F5">
-            <v>13</v>
+            <v>14</v>
           </cell>
           <cell r="G5">
-            <v>7</v>
+            <v>10</v>
           </cell>
           <cell r="H5">
             <v>0</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
@@ -988,6 +1472,50 @@
       <sheetData sheetId="17"/>
       <sheetData sheetId="18"/>
       <sheetData sheetId="19"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sprint1"/>
+      <sheetName val="Burndown1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="3">
+          <cell r="E3" t="str">
+            <v>28/2/2022</v>
+          </cell>
+          <cell r="F3">
+            <v>44621</v>
+          </cell>
+          <cell r="G3">
+            <v>44622</v>
+          </cell>
+          <cell r="H3">
+            <v>44623</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="E5">
+            <v>16</v>
+          </cell>
+          <cell r="F5">
+            <v>14</v>
+          </cell>
+          <cell r="G5">
+            <v>9</v>
+          </cell>
+          <cell r="H5">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1255,11 +1783,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE2AEC1-BBA1-4525-92E0-6A83F17E58C2}">
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,126 +1796,127 @@
     <col min="2" max="2" width="58.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="6"/>
+      <c r="A1" s="31"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="6"/>
+      <c r="I2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="13">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="12">
         <v>44621</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="12">
         <v>44622</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="12">
         <v>44623</v>
       </c>
-      <c r="I3" s="14"/>
+      <c r="I3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15">
         <v>16</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <v>11</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="16">
         <f>6</f>
         <v>6</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="16">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="I4" s="18" t="s">
-        <v>10</v>
+      <c r="I4" s="25" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="15">
+      <c r="A5" s="10"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="14">
         <v>16</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="15">
         <f t="shared" ref="E5:H5" si="0">SUM(E6:E11)</f>
         <v>16</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="16">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="16">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I5" s="18" t="s">
-        <v>11</v>
+      <c r="I5" s="25" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>14</v>
+      <c r="A6" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>10</v>
       </c>
       <c r="D6" s="22">
         <v>4</v>
@@ -1404,15 +1933,15 @@
       <c r="H6" s="24">
         <v>0</v>
       </c>
-      <c r="I6" s="6"/>
+      <c r="I6" s="32"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>16</v>
+      <c r="A7" s="37"/>
+      <c r="B7" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>11</v>
       </c>
       <c r="D7" s="22">
         <v>4</v>
@@ -1429,15 +1958,15 @@
       <c r="H7" s="24">
         <v>0</v>
       </c>
-      <c r="I7" s="6"/>
+      <c r="I7" s="32"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>18</v>
+      <c r="A8" s="37"/>
+      <c r="B8" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>13</v>
       </c>
       <c r="D8" s="22">
         <v>4</v>
@@ -1454,15 +1983,15 @@
       <c r="H8" s="24">
         <v>1</v>
       </c>
-      <c r="I8" s="6"/>
+      <c r="I8" s="32"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>20</v>
+      <c r="A9" s="38"/>
+      <c r="B9" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>15</v>
       </c>
       <c r="D9" s="22">
         <v>4</v>
@@ -1479,151 +2008,151 @@
       <c r="H9" s="24">
         <v>0</v>
       </c>
-      <c r="I9" s="6"/>
+      <c r="I9" s="32"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="6"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="32"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="6"/>
+      <c r="A13" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="32"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="6"/>
+      <c r="A14" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="32"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="6"/>
+      <c r="A15" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="32"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="6"/>
+      <c r="A16" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="32"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="6"/>
+      <c r="A17" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="32"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="6"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="32"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="6"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="32"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="28">
+      <c r="A20" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="30">
         <f>4*4</f>
         <v>16</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="6"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1649,11 +2178,404 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB10B1BA-679F-493B-9865-158A34995B65}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E083C6-746C-42CC-9205-D51AE0B144AA}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="V20" sqref="V20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12">
+        <v>44745</v>
+      </c>
+      <c r="F3" s="13">
+        <v>44776</v>
+      </c>
+      <c r="G3" s="13">
+        <v>44807</v>
+      </c>
+      <c r="H3" s="13">
+        <v>44837</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15">
+        <f>24</f>
+        <v>24</v>
+      </c>
+      <c r="F4" s="16">
+        <f>E4-9</f>
+        <v>15</v>
+      </c>
+      <c r="G4" s="16">
+        <f>F4-8</f>
+        <v>7</v>
+      </c>
+      <c r="H4" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="17"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="14">
+        <v>24</v>
+      </c>
+      <c r="E5" s="15">
+        <f t="shared" ref="E5:H5" si="0">SUM(E6:E9)</f>
+        <v>24</v>
+      </c>
+      <c r="F5" s="16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G5" s="16">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H5" s="16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="22">
+        <v>6</v>
+      </c>
+      <c r="E6" s="23">
+        <v>6</v>
+      </c>
+      <c r="F6" s="24">
+        <v>3</v>
+      </c>
+      <c r="G6" s="24">
+        <v>3</v>
+      </c>
+      <c r="H6" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="22">
+        <v>6</v>
+      </c>
+      <c r="E7" s="23">
+        <v>6</v>
+      </c>
+      <c r="F7" s="24">
+        <v>2</v>
+      </c>
+      <c r="G7" s="24">
+        <v>2</v>
+      </c>
+      <c r="H7" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="22">
+        <v>6</v>
+      </c>
+      <c r="E8" s="23">
+        <v>6</v>
+      </c>
+      <c r="F8" s="24">
+        <v>4</v>
+      </c>
+      <c r="G8" s="24">
+        <v>3</v>
+      </c>
+      <c r="H8" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="22">
+        <v>6</v>
+      </c>
+      <c r="E9" s="23">
+        <v>6</v>
+      </c>
+      <c r="F9" s="24">
+        <v>3</v>
+      </c>
+      <c r="G9" s="24">
+        <v>2</v>
+      </c>
+      <c r="H9" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="30">
+        <f>4*6</f>
+        <v>24</v>
+      </c>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A6:A9"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF57BB8A"/>
+        <color rgb="FFFFFFFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8444963-5411-4FD1-ABF8-DD35E24FFBAE}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated journal & sprint
</commit_message>
<xml_diff>
--- a/HotelBookingApplication/files/Sprint/Sprint.xlsx
+++ b/HotelBookingApplication/files/Sprint/Sprint.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajup\Desktop\Sprint Sheets\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33004647-9FC1-4609-BA52-82895F18126C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE54DDF-7928-4965-A709-CA9F8383E135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-6180" windowWidth="30936" windowHeight="16776" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprint1" sheetId="3" r:id="rId1"/>
-    <sheet name="Burndown1" sheetId="4" r:id="rId2"/>
-    <sheet name="Sprint2" sheetId="1" r:id="rId3"/>
-    <sheet name="Burndown2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sprint1" sheetId="5" r:id="rId1"/>
+    <sheet name="Burndown1" sheetId="6" r:id="rId2"/>
+    <sheet name="Sprint2" sheetId="7" r:id="rId3"/>
+    <sheet name="Burndown2" sheetId="8" r:id="rId4"/>
+    <sheet name="Sprint3" sheetId="1" r:id="rId5"/>
+    <sheet name="Burndown3" sheetId="2" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,102 +44,126 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
+  <si>
+    <t>Week #3  (4 days / week3)</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Task Owner</t>
+  </si>
+  <si>
+    <t>Initial Estimate (Total Sprint Hours = 32*1)</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>Ideal Burndown</t>
+  </si>
+  <si>
+    <t>Remaining Hrs (Total)</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Database Design</t>
+  </si>
+  <si>
+    <t>Akhil</t>
+  </si>
+  <si>
+    <t>Sharan</t>
+  </si>
+  <si>
+    <t>Architecture Diagram</t>
+  </si>
+  <si>
+    <t>Raju</t>
+  </si>
+  <si>
+    <t>Class Diagram</t>
+  </si>
+  <si>
+    <t>Prerna</t>
+  </si>
+  <si>
+    <t>Team:</t>
+  </si>
+  <si>
+    <t>8 hours / Week</t>
+  </si>
+  <si>
+    <t>Total Available Hours During Sprint 3:</t>
+  </si>
+  <si>
+    <t>Total Available Hours During Sprint 1:</t>
+  </si>
+  <si>
+    <t>4 hours / Week</t>
+  </si>
+  <si>
+    <t>Figure out the pages design to be included</t>
+  </si>
+  <si>
+    <t>Figure out the technologies</t>
+  </si>
+  <si>
+    <t>Figure out the components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understand the requirements &amp; explore other hotel sites </t>
+  </si>
+  <si>
+    <t>Requirement Analysis</t>
+  </si>
+  <si>
+    <t>28/2/2022</t>
+  </si>
+  <si>
+    <t>Initial Estimate (Total Sprint Hours = 16*1)</t>
+  </si>
+  <si>
+    <t>Backlog Item</t>
+  </si>
+  <si>
+    <t>Week #1 (4 days / week)</t>
+  </si>
+  <si>
+    <t>Total Available Hours During Sprint 2:</t>
+  </si>
+  <si>
+    <t>6 hours / Week</t>
+  </si>
+  <si>
+    <t>Configure the project tech stack i.e MongoDB</t>
+  </si>
+  <si>
+    <t>Configure the project tech stack i.e ReactJS</t>
+  </si>
+  <si>
+    <t>Configure the project tech stack i.e ReactJS &amp; Node</t>
+  </si>
+  <si>
+    <t>Environment Setup</t>
+  </si>
+  <si>
+    <t>Initial Estimate (Total Sprint Hours = 24*1)</t>
+  </si>
   <si>
     <t>Week #2  (4 days / week)</t>
-  </si>
-  <si>
-    <t>Task</t>
-  </si>
-  <si>
-    <t>Task Owner</t>
-  </si>
-  <si>
-    <t>Initial Estimate (Total Sprint Hours = 24*1)</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>Environment Setup</t>
-  </si>
-  <si>
-    <t>Configure the project tech stack i.e ReactJS &amp; Node</t>
-  </si>
-  <si>
-    <t>Akhil</t>
-  </si>
-  <si>
-    <t>Sharan</t>
-  </si>
-  <si>
-    <t>Configure the project tech stack i.e ReactJS</t>
-  </si>
-  <si>
-    <t>Raju</t>
-  </si>
-  <si>
-    <t>Configure the project tech stack i.e MongoDB</t>
-  </si>
-  <si>
-    <t>Prerna</t>
-  </si>
-  <si>
-    <t>Team:</t>
-  </si>
-  <si>
-    <t>6 hours / Week</t>
-  </si>
-  <si>
-    <t>Total Available Hours During Sprint 2:</t>
-  </si>
-  <si>
-    <t>Week #1 (4 days / week)</t>
-  </si>
-  <si>
-    <t>Backlog Item</t>
-  </si>
-  <si>
-    <t>Initial Estimate (Total Sprint Hours = 16*1)</t>
-  </si>
-  <si>
-    <t>28/2/2022</t>
-  </si>
-  <si>
-    <t>Ideal Burndown</t>
-  </si>
-  <si>
-    <t>Remaining Hrs (Total)</t>
-  </si>
-  <si>
-    <t>Requirement Analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Understand the requirements &amp; explore other hotel sites </t>
-  </si>
-  <si>
-    <t>Figure out the components</t>
-  </si>
-  <si>
-    <t>Figure out the technologies</t>
-  </si>
-  <si>
-    <t>Figure out the pages design to be included</t>
-  </si>
-  <si>
-    <t>4 hours / Week</t>
-  </si>
-  <si>
-    <t>Total Available Hours During Sprint 1:</t>
   </si>
 </sst>
 </file>
@@ -147,7 +173,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m&quot;/&quot;d"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +198,13 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -216,6 +249,7 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -408,10 +442,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
-      </top>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -432,17 +466,17 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="thin">
         <color indexed="64"/>
-      </bottom>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -454,98 +488,104 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -674,7 +714,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5195-4790-91E3-C8D57E4938BB}"/>
+              <c16:uniqueId val="{00000000-9EAE-4BED-97C3-0FDDCEB72F17}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -739,7 +779,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5195-4790-91E3-C8D57E4938BB}"/>
+              <c16:uniqueId val="{00000001-9EAE-4BED-97C3-0FDDCEB72F17}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1038,7 +1078,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7945-45CB-97EB-BCCBC5526564}"/>
+              <c16:uniqueId val="{00000000-A5B3-4436-9509-DC4BB6137D43}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1104,7 +1144,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7945-45CB-97EB-BCCBC5526564}"/>
+              <c16:uniqueId val="{00000001-A5B3-4436-9509-DC4BB6137D43}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1292,6 +1332,370 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1600" b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:rPr>
+              <a:t>Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal Burn Down </c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="3366CC">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sprint3!$E$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>m"/"d</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>44634</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44635</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44636</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44637</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]Sprint3!$E$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DC95-4A04-BE09-6DE4BB95878D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual Burn Down</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="DC3912">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="DC3912"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sprint3!$E$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>m"/"d</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>44634</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44635</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44636</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44637</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint3!$E$5:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DC95-4A04-BE09-6DE4BB95878D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1813899011"/>
+        <c:axId val="428469870"/>
+      </c:areaChart>
+      <c:dateAx>
+        <c:axId val="1813899011"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="m&quot;/&quot;d" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="428469870"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="428469870"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t>Remaining  Hours</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1813899011"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Roboto"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
@@ -1307,7 +1711,7 @@
         <xdr:cNvPr id="2" name="Chart 1" title="Chart">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BFEE298-686C-432C-851C-FA488AB96B2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45DCF71A-21AB-4190-875F-DBC430C55B32}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1345,7 +1749,45 @@
         <xdr:cNvPr id="2" name="Chart 2" title="Chart">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C72E5036-31C6-40F2-BB42-D34BA0D2F7BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A29C2ED-5A11-4914-BD1C-8BAD1A284BAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="9763125" cy="4914900"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 3" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E258383-F52B-4AD5-9C65-B6286A93379B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1412,20 +1854,6 @@
       </sheetData>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2">
-        <row r="3">
-          <cell r="E3">
-            <v>44745</v>
-          </cell>
-          <cell r="F3">
-            <v>44776</v>
-          </cell>
-          <cell r="G3">
-            <v>44807</v>
-          </cell>
-          <cell r="H3">
-            <v>44837</v>
-          </cell>
-        </row>
         <row r="4">
           <cell r="E4">
             <v>24</v>
@@ -1440,23 +1868,52 @@
             <v>0</v>
           </cell>
         </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4">
+        <row r="3">
+          <cell r="E3">
+            <v>44634</v>
+          </cell>
+          <cell r="F3">
+            <v>44635</v>
+          </cell>
+          <cell r="G3">
+            <v>44636</v>
+          </cell>
+          <cell r="H3">
+            <v>44637</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="E4">
+            <v>32</v>
+          </cell>
+          <cell r="F4">
+            <v>21</v>
+          </cell>
+          <cell r="G4">
+            <v>10</v>
+          </cell>
+          <cell r="H4">
+            <v>0</v>
+          </cell>
+        </row>
         <row r="5">
           <cell r="E5">
-            <v>24</v>
+            <v>29</v>
           </cell>
           <cell r="F5">
-            <v>14</v>
+            <v>19</v>
           </cell>
           <cell r="G5">
-            <v>10</v>
+            <v>9</v>
           </cell>
           <cell r="H5">
             <v>0</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
@@ -1783,7 +2240,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE2AEC1-BBA1-4525-92E0-6A83F17E58C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D18D23B-50CF-4C3C-B5E9-7AF9823A643C}">
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1800,368 +2257,368 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="31"/>
+      <c r="A1" s="39"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
-      <c r="I1" s="32"/>
+      <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="32"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="12">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="13">
         <v>44621</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="13">
         <v>44622</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="13">
         <v>44623</v>
       </c>
-      <c r="I3" s="33"/>
+      <c r="I3" s="15"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17">
         <v>16</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="18">
         <v>11</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="18">
         <f>6</f>
         <v>6</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="18">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="I4" s="25" t="s">
-        <v>23</v>
+      <c r="I4" s="19" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="14">
+      <c r="A5" s="11"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="16">
         <v>16</v>
       </c>
-      <c r="E5" s="15">
-        <f t="shared" ref="E5:H5" si="0">SUM(E6:E11)</f>
+      <c r="E5" s="17">
+        <f>SUM(E6:E11)</f>
         <v>16</v>
       </c>
-      <c r="F5" s="16">
-        <f t="shared" si="0"/>
+      <c r="F5" s="18">
+        <f>SUM(F6:F11)</f>
         <v>14</v>
       </c>
-      <c r="G5" s="16">
-        <f t="shared" si="0"/>
+      <c r="G5" s="18">
+        <f>SUM(G6:G11)</f>
         <v>9</v>
       </c>
-      <c r="H5" s="16">
-        <f t="shared" si="0"/>
+      <c r="H5" s="18">
+        <f>SUM(H6:H11)</f>
         <v>1</v>
       </c>
-      <c r="I5" s="25" t="s">
-        <v>24</v>
+      <c r="I5" s="19" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
-        <v>25</v>
+      <c r="A6" s="38" t="s">
+        <v>27</v>
       </c>
       <c r="B6" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="22">
+      <c r="C6" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="25">
         <v>4</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="26">
         <v>4</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="27">
         <v>4</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="27">
         <v>3</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="27">
         <v>0</v>
       </c>
-      <c r="I6" s="32"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="37"/>
       <c r="B7" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="22">
+        <v>25</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="25">
         <v>4</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="26">
         <v>4</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="27">
         <v>3</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="27">
         <v>2</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="27">
         <v>0</v>
       </c>
-      <c r="I7" s="32"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="37"/>
       <c r="B8" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="25">
+        <v>4</v>
+      </c>
+      <c r="E8" s="26">
+        <v>4</v>
+      </c>
+      <c r="F8" s="27">
+        <v>4</v>
+      </c>
+      <c r="G8" s="27">
+        <v>0</v>
+      </c>
+      <c r="H8" s="27">
+        <v>1</v>
+      </c>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="36"/>
+      <c r="B9" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="25">
+        <v>4</v>
+      </c>
+      <c r="E9" s="26">
+        <v>4</v>
+      </c>
+      <c r="F9" s="27">
+        <v>3</v>
+      </c>
+      <c r="G9" s="27">
+        <v>4</v>
+      </c>
+      <c r="H9" s="27">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="22">
-        <v>4</v>
-      </c>
-      <c r="E8" s="23">
-        <v>4</v>
-      </c>
-      <c r="F8" s="24">
-        <v>4</v>
-      </c>
-      <c r="G8" s="24">
-        <v>0</v>
-      </c>
-      <c r="H8" s="24">
-        <v>1</v>
-      </c>
-      <c r="I8" s="32"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="36" t="s">
+      <c r="B15" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="22">
-        <v>4</v>
-      </c>
-      <c r="E9" s="23">
-        <v>4</v>
-      </c>
-      <c r="F9" s="24">
-        <v>3</v>
-      </c>
-      <c r="G9" s="24">
-        <v>4</v>
-      </c>
-      <c r="H9" s="24">
-        <v>0</v>
-      </c>
-      <c r="I9" s="32"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="32"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="32"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="32"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="32"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="32"/>
+      <c r="B16" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="32"/>
+      <c r="A17" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="32"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="32"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="30">
+      <c r="A20" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="32">
         <f>4*4</f>
         <v>16</v>
       </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="32"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A6:A9"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="D2:D3"/>
-    <mergeCell ref="A6:A9"/>
   </mergeCells>
   <conditionalFormatting sqref="A6">
     <cfRule type="colorScale" priority="1">
@@ -2178,10 +2635,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E083C6-746C-42CC-9205-D51AE0B144AA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A98503B7-6D3F-40EE-9281-BA03E6B3264A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
@@ -2193,7 +2650,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF45CCF-906A-4C74-9279-87E54946CEAE}">
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2214,339 +2671,339 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12">
+      <c r="A3" s="6"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13">
         <v>44745</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="14">
         <v>44776</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="14">
         <v>44807</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="14">
         <v>44837</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15">
+      <c r="A4" s="6"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17">
         <f>24</f>
         <v>24</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="18">
         <f>E4-9</f>
         <v>15</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="18">
         <f>F4-8</f>
         <v>7</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="14">
+      <c r="A5" s="20"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="16">
         <v>24</v>
       </c>
-      <c r="E5" s="15">
-        <f t="shared" ref="E5:H5" si="0">SUM(E6:E9)</f>
+      <c r="E5" s="17">
+        <f>SUM(E6:E9)</f>
         <v>24</v>
       </c>
-      <c r="F5" s="16">
-        <f t="shared" si="0"/>
+      <c r="F5" s="18">
+        <f>SUM(F6:F9)</f>
         <v>12</v>
       </c>
-      <c r="G5" s="16">
-        <f t="shared" si="0"/>
+      <c r="G5" s="18">
+        <f>SUM(G6:G9)</f>
         <v>10</v>
       </c>
-      <c r="H5" s="16">
-        <f t="shared" si="0"/>
+      <c r="H5" s="18">
+        <f>SUM(H6:H9)</f>
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="22">
+      <c r="A6" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="25">
         <v>6</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="26">
         <v>6</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="27">
         <v>3</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="27">
         <v>3</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="22">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="25">
         <v>6</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="26">
         <v>6</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="27">
         <v>2</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="27">
         <v>2</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="27">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="25">
+        <v>6</v>
+      </c>
+      <c r="E8" s="26">
+        <v>6</v>
+      </c>
+      <c r="F8" s="27">
+        <v>4</v>
+      </c>
+      <c r="G8" s="27">
+        <v>3</v>
+      </c>
+      <c r="H8" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="25">
+        <v>6</v>
+      </c>
+      <c r="E9" s="26">
+        <v>6</v>
+      </c>
+      <c r="F9" s="27">
+        <v>3</v>
+      </c>
+      <c r="G9" s="27">
+        <v>2</v>
+      </c>
+      <c r="H9" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="B15" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="22">
-        <v>6</v>
-      </c>
-      <c r="E8" s="23">
-        <v>6</v>
-      </c>
-      <c r="F8" s="24">
-        <v>4</v>
-      </c>
-      <c r="G8" s="24">
-        <v>3</v>
-      </c>
-      <c r="H8" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="21" t="s">
+      <c r="B16" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="22">
-        <v>6</v>
-      </c>
-      <c r="E9" s="23">
-        <v>6</v>
-      </c>
-      <c r="F9" s="24">
-        <v>3</v>
-      </c>
-      <c r="G9" s="24">
-        <v>2</v>
-      </c>
-      <c r="H9" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="26" t="s">
+      <c r="B17" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
+      <c r="B18" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="30">
+      <c r="A21" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="32">
         <f>4*6</f>
         <v>24</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2571,11 +3028,428 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8444963-5411-4FD1-ABF8-DD35E24FFBAE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A728917-8F4F-4FCB-9E56-7F439F120389}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+      <selection activeCell="J38" sqref="J38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13">
+        <v>44634</v>
+      </c>
+      <c r="F3" s="14">
+        <v>44635</v>
+      </c>
+      <c r="G3" s="14">
+        <v>44636</v>
+      </c>
+      <c r="H3" s="14">
+        <v>44637</v>
+      </c>
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17">
+        <f>32</f>
+        <v>32</v>
+      </c>
+      <c r="F4" s="18">
+        <f t="shared" ref="F4:G4" si="0">E4-11</f>
+        <v>21</v>
+      </c>
+      <c r="G4" s="18">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H4" s="18">
+        <v>0</v>
+      </c>
+      <c r="I4" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="16">
+        <v>32</v>
+      </c>
+      <c r="E5" s="17">
+        <f t="shared" ref="E5:G5" si="1">SUM(E6:E10)</f>
+        <v>29</v>
+      </c>
+      <c r="F5" s="18">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="G5" s="18">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="H5" s="18">
+        <f>SUM(H6:H9)</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="25">
+        <v>8</v>
+      </c>
+      <c r="E6" s="26">
+        <v>8</v>
+      </c>
+      <c r="F6" s="27">
+        <v>6</v>
+      </c>
+      <c r="G6" s="27">
+        <v>3</v>
+      </c>
+      <c r="H6" s="27">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+      <c r="B7" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="25">
+        <v>8</v>
+      </c>
+      <c r="E7" s="26">
+        <v>8</v>
+      </c>
+      <c r="F7" s="27">
+        <v>5</v>
+      </c>
+      <c r="G7" s="27">
+        <v>2</v>
+      </c>
+      <c r="H7" s="27">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+      <c r="B8" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="25">
+        <v>8</v>
+      </c>
+      <c r="E8" s="26">
+        <v>8</v>
+      </c>
+      <c r="F8" s="27">
+        <v>4</v>
+      </c>
+      <c r="G8" s="27">
+        <v>3</v>
+      </c>
+      <c r="H8" s="27">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="25">
+        <v>8</v>
+      </c>
+      <c r="E9" s="26">
+        <v>5</v>
+      </c>
+      <c r="F9" s="27">
+        <v>4</v>
+      </c>
+      <c r="G9" s="27">
+        <v>1</v>
+      </c>
+      <c r="H9" s="27">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="19"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="29"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="33">
+        <v>32</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A6:A9"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF57BB8A"/>
+        <color rgb="FFFFFFFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DDC2D45-B214-47E3-B816-08B7A65968C9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Journal & Sprint for 4th week
</commit_message>
<xml_diff>
--- a/HotelBookingApplication/files/Sprint/Sprint.xlsx
+++ b/HotelBookingApplication/files/Sprint/Sprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajup\Desktop\Sprint Sheets\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE54DDF-7928-4965-A709-CA9F8383E135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4081E924-A296-4846-B64A-13ED5DB9A3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-6180" windowWidth="30936" windowHeight="16776" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-6180" windowWidth="30936" windowHeight="16776" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="5" r:id="rId1"/>
@@ -19,10 +19,12 @@
     <sheet name="Burndown2" sheetId="8" r:id="rId4"/>
     <sheet name="Sprint3" sheetId="1" r:id="rId5"/>
     <sheet name="Burndown3" sheetId="2" r:id="rId6"/>
+    <sheet name="Sprint4" sheetId="9" r:id="rId7"/>
+    <sheet name="Burndown4" sheetId="10" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="46">
   <si>
     <t>Week #3  (4 days / week3)</t>
   </si>
@@ -164,6 +166,24 @@
   </si>
   <si>
     <t>Week #2  (4 days / week)</t>
+  </si>
+  <si>
+    <t>Initial components setup, creating wireframes and basic logic implementation</t>
+  </si>
+  <si>
+    <t>Search API</t>
+  </si>
+  <si>
+    <t>Holiday &amp; Weekend Pricing</t>
+  </si>
+  <si>
+    <t>Sign Up &amp; Login API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design wireframes for Sign Up &amp; Login </t>
+  </si>
+  <si>
+    <t>Total Available Hours During Sprint 4:</t>
   </si>
 </sst>
 </file>
@@ -173,7 +193,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m&quot;/&quot;d"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +276,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -277,7 +303,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -472,11 +498,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF0000FF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -587,6 +626,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1696,6 +1756,371 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1600" b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:rPr>
+              <a:t>Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal Burn Down </c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="3366CC">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sprint4!$E$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint4!$E$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8B2E-4493-8155-BFBBDE5270D7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual Burn Down</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="DC3912">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="DC3912"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sprint4!$E$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint4!$E$5:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8B2E-4493-8155-BFBBDE5270D7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1868032141"/>
+        <c:axId val="1310802712"/>
+      </c:areaChart>
+      <c:catAx>
+        <c:axId val="1868032141"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1310802712"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1310802712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t>Remaining  Hours</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1868032141"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Roboto"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
@@ -1788,6 +2213,44 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E258383-F52B-4AD5-9C65-B6286A93379B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="9763125" cy="4914900"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 4" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47948AFC-3B42-44B1-9147-CEDBF1C4E419}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1915,7 +2378,50 @@
         </row>
       </sheetData>
       <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
+      <sheetData sheetId="6">
+        <row r="3">
+          <cell r="E3">
+            <v>44672</v>
+          </cell>
+          <cell r="F3">
+            <v>44673</v>
+          </cell>
+          <cell r="G3">
+            <v>44674</v>
+          </cell>
+          <cell r="H3">
+            <v>44675</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="E4">
+            <v>32</v>
+          </cell>
+          <cell r="F4">
+            <v>22</v>
+          </cell>
+          <cell r="G4">
+            <v>12</v>
+          </cell>
+          <cell r="H4">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="E5">
+            <v>25</v>
+          </cell>
+          <cell r="F5">
+            <v>18</v>
+          </cell>
+          <cell r="G5">
+            <v>9</v>
+          </cell>
+          <cell r="H5">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
@@ -3046,7 +3552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -3457,4 +3963,291 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A89C13D9-BF48-4209-952E-8CD36B152D9A}">
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.5703125" customWidth="1"/>
+    <col min="2" max="2" width="41.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13">
+        <v>44672</v>
+      </c>
+      <c r="F2" s="14">
+        <v>44673</v>
+      </c>
+      <c r="G2" s="14">
+        <v>44674</v>
+      </c>
+      <c r="H2" s="14">
+        <v>44675</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="17">
+        <f>32</f>
+        <v>32</v>
+      </c>
+      <c r="F3" s="18">
+        <f t="shared" ref="F3:G3" si="0">E3-10</f>
+        <v>22</v>
+      </c>
+      <c r="G3" s="18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H3" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="43">
+        <v>32</v>
+      </c>
+      <c r="E4" s="44">
+        <f>SUM(E5:E10)</f>
+        <v>25</v>
+      </c>
+      <c r="F4" s="45">
+        <f>SUM(F5:F10)</f>
+        <v>18</v>
+      </c>
+      <c r="G4" s="45">
+        <f>SUM(G5:G10)</f>
+        <v>9</v>
+      </c>
+      <c r="H4" s="45">
+        <f>SUM(H5:H10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="41">
+        <v>8</v>
+      </c>
+      <c r="E5" s="42">
+        <v>8</v>
+      </c>
+      <c r="F5" s="42">
+        <v>6</v>
+      </c>
+      <c r="G5" s="42">
+        <v>2</v>
+      </c>
+      <c r="H5" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="46"/>
+      <c r="B6" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="41">
+        <v>8</v>
+      </c>
+      <c r="E6" s="42">
+        <v>5</v>
+      </c>
+      <c r="F6" s="42">
+        <v>3</v>
+      </c>
+      <c r="G6" s="42">
+        <v>2</v>
+      </c>
+      <c r="H6" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="46"/>
+      <c r="B7" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="41">
+        <v>4</v>
+      </c>
+      <c r="E7" s="42">
+        <v>4</v>
+      </c>
+      <c r="F7" s="42">
+        <v>4</v>
+      </c>
+      <c r="G7" s="42">
+        <v>2</v>
+      </c>
+      <c r="H7" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="46"/>
+      <c r="B8" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="41">
+        <v>8</v>
+      </c>
+      <c r="E8" s="42">
+        <v>8</v>
+      </c>
+      <c r="F8" s="42">
+        <v>5</v>
+      </c>
+      <c r="G8" s="42">
+        <v>3</v>
+      </c>
+      <c r="H8" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="47"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="32">
+        <f>4*8</f>
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A5:A8"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A5">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF57BB8A"/>
+        <color rgb="FFFFFFFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60FEA136-E296-43BA-B2A1-5D99FD250533}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U25" sqref="U25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated sprint & journal for 6th week
</commit_message>
<xml_diff>
--- a/HotelBookingApplication/files/Sprint/Sprint.xlsx
+++ b/HotelBookingApplication/files/Sprint/Sprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajup\Desktop\Sprint Sheets\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6F6BAF6-8BA5-440E-BF07-49537278A913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9549C87-8996-4956-8F0B-F7AA53364D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-6180" windowWidth="30936" windowHeight="16776" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-6180" windowWidth="30936" windowHeight="16776" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="5" r:id="rId1"/>
@@ -23,10 +23,12 @@
     <sheet name="Burndown4" sheetId="10" r:id="rId8"/>
     <sheet name="Sprint5" sheetId="12" r:id="rId9"/>
     <sheet name="Burndown5" sheetId="13" r:id="rId10"/>
+    <sheet name="Sprint6" sheetId="15" r:id="rId11"/>
+    <sheet name="Burndown6" sheetId="14" r:id="rId12"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId11"/>
-    <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
+    <externalReference r:id="rId14"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="59">
   <si>
     <t>Week #3  (4 days / week3)</t>
   </si>
@@ -207,6 +209,24 @@
   </si>
   <si>
     <t>Total Available Hours During Sprint 5:</t>
+  </si>
+  <si>
+    <t>Week #6  (4 days / week)</t>
+  </si>
+  <si>
+    <t>UI for Admin, Room &amp; User Profile</t>
+  </si>
+  <si>
+    <t>Admin UI</t>
+  </si>
+  <si>
+    <t>Room UI</t>
+  </si>
+  <si>
+    <t>User Profile UI</t>
+  </si>
+  <si>
+    <t>User Profile Wireframe</t>
   </si>
 </sst>
 </file>
@@ -538,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -671,6 +691,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2509,6 +2532,370 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1600" b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:rPr>
+              <a:t>Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal Burn Down </c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="3366CC">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sprint6!$E$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>m"/"d</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>44655</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44656</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44657</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44658</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint6!$E$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2A0D-4340-A7D3-EE4AE9D45951}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual Burn Down</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="DC3912">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="DC3912"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sprint6!$E$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>m"/"d</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>44655</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44656</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44657</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44658</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint6!$E$5:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2A0D-4340-A7D3-EE4AE9D45951}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1749025759"/>
+        <c:axId val="294563099"/>
+      </c:areaChart>
+      <c:dateAx>
+        <c:axId val="1749025759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="m&quot;/&quot;d" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="294563099"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="294563099"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t>Remaining  Hours</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1749025759"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Roboto"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
@@ -2699,6 +3086,44 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="9763125" cy="4914900"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 6" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F866FC03-9D9C-4A91-88D0-47F9E11E3733}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -2894,7 +3319,50 @@
         </row>
       </sheetData>
       <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
+      <sheetData sheetId="10">
+        <row r="3">
+          <cell r="E3">
+            <v>44655</v>
+          </cell>
+          <cell r="F3">
+            <v>44656</v>
+          </cell>
+          <cell r="G3">
+            <v>44657</v>
+          </cell>
+          <cell r="H3">
+            <v>44658</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="E4">
+            <v>32</v>
+          </cell>
+          <cell r="F4">
+            <v>22</v>
+          </cell>
+          <cell r="G4">
+            <v>12</v>
+          </cell>
+          <cell r="H4">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="E5">
+            <v>32</v>
+          </cell>
+          <cell r="F5">
+            <v>21</v>
+          </cell>
+          <cell r="G5">
+            <v>8</v>
+          </cell>
+          <cell r="H5">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="11"/>
       <sheetData sheetId="12"/>
       <sheetData sheetId="13"/>
@@ -3624,6 +4092,317 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D352693-F578-41E2-BE89-3AAAEC47269D}">
+  <dimension ref="A1:H27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13">
+        <v>44655</v>
+      </c>
+      <c r="F3" s="14">
+        <v>44656</v>
+      </c>
+      <c r="G3" s="14">
+        <v>44657</v>
+      </c>
+      <c r="H3" s="14">
+        <v>44658</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17">
+        <f>32</f>
+        <v>32</v>
+      </c>
+      <c r="F4" s="18">
+        <f t="shared" ref="F4:G4" si="0">E4-10</f>
+        <v>22</v>
+      </c>
+      <c r="G4" s="18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H4" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="16">
+        <v>32</v>
+      </c>
+      <c r="E5" s="17">
+        <f>SUM(E6:E9)</f>
+        <v>32</v>
+      </c>
+      <c r="F5" s="18">
+        <f>SUM(F6:F9)</f>
+        <v>21</v>
+      </c>
+      <c r="G5" s="18">
+        <f>SUM(G6:G9)</f>
+        <v>8</v>
+      </c>
+      <c r="H5" s="18">
+        <f>SUM(H8:H9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="25">
+        <v>8</v>
+      </c>
+      <c r="E6" s="26">
+        <v>8</v>
+      </c>
+      <c r="F6" s="27">
+        <v>5</v>
+      </c>
+      <c r="G6" s="27">
+        <v>2</v>
+      </c>
+      <c r="H6" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="47"/>
+      <c r="B7" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="25">
+        <v>8</v>
+      </c>
+      <c r="E7" s="26">
+        <v>8</v>
+      </c>
+      <c r="F7" s="27">
+        <v>7</v>
+      </c>
+      <c r="G7" s="27">
+        <v>3</v>
+      </c>
+      <c r="H7" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="47"/>
+      <c r="B8" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="25">
+        <v>8</v>
+      </c>
+      <c r="E8" s="26">
+        <v>8</v>
+      </c>
+      <c r="F8" s="27">
+        <v>4</v>
+      </c>
+      <c r="G8" s="27">
+        <v>1</v>
+      </c>
+      <c r="H8" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="47"/>
+      <c r="B9" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="25">
+        <v>8</v>
+      </c>
+      <c r="E9" s="26">
+        <v>8</v>
+      </c>
+      <c r="F9" s="27">
+        <v>5</v>
+      </c>
+      <c r="G9" s="27">
+        <v>2</v>
+      </c>
+      <c r="H9" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="48"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="48"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="29"/>
+      <c r="B21" s="48"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="48"/>
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="32">
+        <f>4*8</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A6:A9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70006A23-F0D2-44F1-AFD4-4E5765787C9C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A98503B7-6D3F-40EE-9281-BA03E6B3264A}">
   <dimension ref="A1"/>
@@ -4740,7 +5519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E003B168-A9F9-4C49-8B30-065B7A7D99C0}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added 8th sprint & journal
</commit_message>
<xml_diff>
--- a/HotelBookingApplication/files/Sprint/Sprint.xlsx
+++ b/HotelBookingApplication/files/Sprint/Sprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajup\Desktop\Sprint Sheets\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C1F641-E334-46D7-B55B-A62B48C03195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF00613C-0B5B-4D08-81E8-B5B110F1ED3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-6180" windowWidth="30936" windowHeight="16776" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-6180" windowWidth="30936" windowHeight="16776" firstSheet="3" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="5" r:id="rId1"/>
@@ -27,10 +27,12 @@
     <sheet name="Burndown6" sheetId="14" r:id="rId12"/>
     <sheet name="Sprint7" sheetId="16" r:id="rId13"/>
     <sheet name="Burndown7" sheetId="17" r:id="rId14"/>
+    <sheet name="Sprint8" sheetId="19" r:id="rId15"/>
+    <sheet name="Burndown8" sheetId="20" r:id="rId16"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId15"/>
-    <externalReference r:id="rId16"/>
+    <externalReference r:id="rId17"/>
+    <externalReference r:id="rId18"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="71">
   <si>
     <t>Week #3  (4 days / week3)</t>
   </si>
@@ -250,6 +252,21 @@
   </si>
   <si>
     <t>Total Available Hours During Sprint 7:</t>
+  </si>
+  <si>
+    <t>Week #8  (4 days / week)</t>
+  </si>
+  <si>
+    <t>Testing &amp; Bug Fixing</t>
+  </si>
+  <si>
+    <t>Bug Fixing</t>
+  </si>
+  <si>
+    <t>AWS Deployment Information</t>
+  </si>
+  <si>
+    <t>Total Available Hours During Sprint 8:</t>
   </si>
 </sst>
 </file>
@@ -635,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -809,6 +826,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3339,6 +3360,370 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="637951166"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Roboto"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1600" b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:rPr>
+              <a:t>Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal Burn Down </c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="3366CC">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sprint8!$E$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>m"/"d</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>44669</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44670</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44671</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44672</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint8!$E$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9E2E-489F-B7E5-AAEC449F949E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual Burn Down</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="DC3912">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="DC3912"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sprint8!$E$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>m"/"d</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>44669</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44670</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44671</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44672</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint8!$E$5:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9E2E-489F-B7E5-AAEC449F949E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1315619328"/>
+        <c:axId val="33871973"/>
+      </c:areaChart>
+      <c:dateAx>
+        <c:axId val="1315619328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="m&quot;/&quot;d" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="33871973"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="33871973"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t>Remaining  Hours</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1315619328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3640,6 +4025,44 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="9763125" cy="4914900"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 8" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DE105A6-BF43-49AC-9346-BB1648308BEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -3925,7 +4348,50 @@
         </row>
       </sheetData>
       <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
+      <sheetData sheetId="14">
+        <row r="3">
+          <cell r="E3">
+            <v>44669</v>
+          </cell>
+          <cell r="F3">
+            <v>44670</v>
+          </cell>
+          <cell r="G3">
+            <v>44671</v>
+          </cell>
+          <cell r="H3">
+            <v>44672</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="E4">
+            <v>32</v>
+          </cell>
+          <cell r="F4">
+            <v>22</v>
+          </cell>
+          <cell r="G4">
+            <v>12</v>
+          </cell>
+          <cell r="H4">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="E5">
+            <v>32</v>
+          </cell>
+          <cell r="F5">
+            <v>19</v>
+          </cell>
+          <cell r="G5">
+            <v>12</v>
+          </cell>
+          <cell r="H5">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="15"/>
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
@@ -4966,8 +5432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93034AA3-354E-4870-929C-A07360F96334}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" activeCellId="1" sqref="D24 F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5372,6 +5838,397 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C29DED3-C983-4757-85DD-2335C9DF4D8A}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13">
+        <v>44669</v>
+      </c>
+      <c r="F3" s="14">
+        <v>44670</v>
+      </c>
+      <c r="G3" s="14">
+        <v>44671</v>
+      </c>
+      <c r="H3" s="14">
+        <v>44672</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17">
+        <f>32</f>
+        <v>32</v>
+      </c>
+      <c r="F4" s="18">
+        <f t="shared" ref="F4:G4" si="0">E4-10</f>
+        <v>22</v>
+      </c>
+      <c r="G4" s="18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H4" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="16">
+        <v>32</v>
+      </c>
+      <c r="E5" s="17">
+        <f>SUM(E6:E9)</f>
+        <v>32</v>
+      </c>
+      <c r="F5" s="18">
+        <f>SUM(F6:F9)</f>
+        <v>19</v>
+      </c>
+      <c r="G5" s="18">
+        <f>SUM(G6:G9)</f>
+        <v>12</v>
+      </c>
+      <c r="H5" s="18">
+        <f>SUM(H7:H9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="67" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="25">
+        <v>8</v>
+      </c>
+      <c r="E6" s="26">
+        <v>8</v>
+      </c>
+      <c r="F6" s="27">
+        <v>7</v>
+      </c>
+      <c r="G6" s="27">
+        <v>3</v>
+      </c>
+      <c r="H6" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="68"/>
+      <c r="B7" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="25">
+        <v>8</v>
+      </c>
+      <c r="E7" s="26">
+        <v>8</v>
+      </c>
+      <c r="F7" s="27">
+        <v>4</v>
+      </c>
+      <c r="G7" s="27">
+        <v>3</v>
+      </c>
+      <c r="H7" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="68"/>
+      <c r="B8" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="25">
+        <v>8</v>
+      </c>
+      <c r="E8" s="26">
+        <v>8</v>
+      </c>
+      <c r="F8" s="27">
+        <v>4</v>
+      </c>
+      <c r="G8" s="27">
+        <v>2</v>
+      </c>
+      <c r="H8" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="68"/>
+      <c r="B9" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="25">
+        <v>8</v>
+      </c>
+      <c r="E9" s="26">
+        <v>8</v>
+      </c>
+      <c r="F9" s="27">
+        <v>4</v>
+      </c>
+      <c r="G9" s="27">
+        <v>4</v>
+      </c>
+      <c r="H9" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="29"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="48"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="32">
+        <f>4*8</f>
+        <v>32</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A6:A9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772113C1-7552-41C6-AB54-36607AED73C5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated final scrum & journal
</commit_message>
<xml_diff>
--- a/HotelBookingApplication/files/Sprint/Sprint.xlsx
+++ b/HotelBookingApplication/files/Sprint/Sprint.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajup\Desktop\Sprint Sheets\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF00613C-0B5B-4D08-81E8-B5B110F1ED3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E8FE77-1C7E-43B4-AB23-3DAB232C6E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-6180" windowWidth="30936" windowHeight="16776" firstSheet="3" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-6180" windowWidth="30936" windowHeight="16776" firstSheet="5" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint1" sheetId="5" r:id="rId1"/>
@@ -29,10 +29,12 @@
     <sheet name="Burndown7" sheetId="17" r:id="rId14"/>
     <sheet name="Sprint8" sheetId="19" r:id="rId15"/>
     <sheet name="Burndown8" sheetId="20" r:id="rId16"/>
+    <sheet name="Sprint9" sheetId="21" r:id="rId17"/>
+    <sheet name="Burndown9" sheetId="22" r:id="rId18"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId17"/>
-    <externalReference r:id="rId18"/>
+    <externalReference r:id="rId19"/>
+    <externalReference r:id="rId20"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="75">
   <si>
     <t>Week #3  (4 days / week3)</t>
   </si>
@@ -267,6 +269,18 @@
   </si>
   <si>
     <t>Total Available Hours During Sprint 8:</t>
+  </si>
+  <si>
+    <t>Week #9  (4 days / week)</t>
+  </si>
+  <si>
+    <t>Deployment setup</t>
+  </si>
+  <si>
+    <t>Deployment</t>
+  </si>
+  <si>
+    <t>Total Available Hours During Sprint 9:</t>
   </si>
 </sst>
 </file>
@@ -3759,6 +3773,370 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr sz="1600" b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:rPr>
+              <a:t>Burndown Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Ideal Burn Down </c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="3366CC">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="3366CC"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sprint9!$E$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>m"/"d</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>44676</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44677</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44678</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44679</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]Sprint8!$E$4:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-816E-4376-9FEC-506F57BE3984}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual Burn Down</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="DC3912">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="DC3912"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sprint9!$E$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>m"/"d</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>44676</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44677</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44678</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44679</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint9!$E$5:$H$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-816E-4376-9FEC-506F57BE3984}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="114947229"/>
+        <c:axId val="1354856419"/>
+      </c:areaChart>
+      <c:dateAx>
+        <c:axId val="114947229"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="m&quot;/&quot;d" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1354856419"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="1354856419"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="0" i="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Roboto"/>
+                  </a:rPr>
+                  <a:t>Remaining  Hours</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0" i="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Roboto"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="114947229"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0" i="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Roboto"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
@@ -4063,6 +4441,44 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="9763125" cy="4914900"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 9" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13A0AC2C-9514-495A-9043-DDCEEC184E4B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -6228,8 +6644,399 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772113C1-7552-41C6-AB54-36607AED73C5}">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F781F5D-4AF6-4E17-8D1E-8C3695F22DB1}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13">
+        <v>44676</v>
+      </c>
+      <c r="F3" s="14">
+        <v>44677</v>
+      </c>
+      <c r="G3" s="14">
+        <v>44678</v>
+      </c>
+      <c r="H3" s="14">
+        <v>44679</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="17">
+        <f>32</f>
+        <v>32</v>
+      </c>
+      <c r="F4" s="18">
+        <f t="shared" ref="F4:G4" si="0">E4-10</f>
+        <v>22</v>
+      </c>
+      <c r="G4" s="18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H4" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="16">
+        <v>32</v>
+      </c>
+      <c r="E5" s="17">
+        <f t="shared" ref="E5:G5" si="1">SUM(E6:E9)</f>
+        <v>32</v>
+      </c>
+      <c r="F5" s="18">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="G5" s="18">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="H5" s="18">
+        <f>SUM(H7:H9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="25">
+        <v>8</v>
+      </c>
+      <c r="E6" s="26">
+        <v>8</v>
+      </c>
+      <c r="F6" s="27">
+        <v>4</v>
+      </c>
+      <c r="G6" s="27">
+        <v>3</v>
+      </c>
+      <c r="H6" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="68"/>
+      <c r="B7" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="25">
+        <v>8</v>
+      </c>
+      <c r="E7" s="26">
+        <v>8</v>
+      </c>
+      <c r="F7" s="27">
+        <v>5</v>
+      </c>
+      <c r="G7" s="27">
+        <v>3</v>
+      </c>
+      <c r="H7" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="68"/>
+      <c r="B8" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="25">
+        <v>8</v>
+      </c>
+      <c r="E8" s="26">
+        <v>8</v>
+      </c>
+      <c r="F8" s="27">
+        <v>4</v>
+      </c>
+      <c r="G8" s="27">
+        <v>4</v>
+      </c>
+      <c r="H8" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="68"/>
+      <c r="B9" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="25">
+        <v>8</v>
+      </c>
+      <c r="E9" s="26">
+        <v>8</v>
+      </c>
+      <c r="F9" s="27">
+        <v>5</v>
+      </c>
+      <c r="G9" s="27">
+        <v>3</v>
+      </c>
+      <c r="H9" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="48"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="48"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="48"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="29"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="48"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="32">
+        <f>4*8</f>
+        <v>32</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A6:A9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53ECF2C3-05FF-4B1D-B839-AF245B64B38A}">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>